<commit_message>
Control de versiones mejorado
</commit_message>
<xml_diff>
--- a/TermicoElectrico.xlsx
+++ b/TermicoElectrico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alonso\OneDrive\OneDrive - UVa\Desktop\CosasAlonso\2024ACTIVIDADES\clase40\2C\DPSE\REPO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvaes-my.sharepoint.com/personal/mario_medrano_estudiantes_uva_es/Documents/Universidad/4/DPSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F9DACCD-BCF0-4C6B-8B1D-F9FF34E58E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{1F9DACCD-BCF0-4C6B-8B1D-F9FF34E58E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDCD4865-34BE-8841-AFEE-80FE280379FF}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2280" windowWidth="21600" windowHeight="11295" xr2:uid="{647B0613-BD7E-4F22-B952-2F2303409225}"/>
+    <workbookView xWindow="7200" yWindow="2280" windowWidth="24740" windowHeight="15240" xr2:uid="{647B0613-BD7E-4F22-B952-2F2303409225}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
-  <si>
-    <t>POWER CALCULATIONS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>COMPONENT</t>
   </si>
@@ -47,9 +44,6 @@
     <t>CONDITIONS</t>
   </si>
   <si>
-    <t>VOLTAGE(Volt)</t>
-  </si>
-  <si>
     <t>LPC2106</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>MPC738321</t>
   </si>
   <si>
-    <t>THERMAL ANALYSIS</t>
-  </si>
-  <si>
     <t>POWER(Watts)</t>
   </si>
   <si>
@@ -147,13 +138,28 @@
   </si>
   <si>
     <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Voltage(Volt)</t>
+  </si>
+  <si>
+    <t>Power Calculations</t>
+  </si>
+  <si>
+    <t>Thermal Analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +173,21 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -190,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -211,6 +232,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -226,10 +249,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,48 +570,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C78B08E-074B-4A43-922D-E89E427C9D01}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C4">
         <v>1.8</v>
@@ -605,10 +624,10 @@
         <v>7.2000000000000008E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1.8</v>
@@ -621,10 +640,10 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1.8</v>
@@ -637,21 +656,21 @@
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>3.3</v>
@@ -665,10 +684,10 @@
         <v>0.18809999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>3.3</v>
@@ -681,18 +700,18 @@
         <v>7.2599999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>3.3</v>
@@ -705,9 +724,9 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>3.3</v>
@@ -720,12 +739,12 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>3.3</v>
@@ -738,20 +757,20 @@
         <v>0.61049999999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>3.7</v>
@@ -765,10 +784,10 @@
         <v>1.0175000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>3.7</v>
@@ -781,18 +800,18 @@
         <v>0.81400000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -805,9 +824,9 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -820,9 +839,9 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -835,75 +854,80 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B29" t="s">
+      <c r="F29" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="4">
         <f>SUM(E4)</f>
         <v>7.2000000000000008E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31" s="4">
         <f>SUM(E5)</f>
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C32" s="4">
         <f>SUM(E6)</f>
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C34" s="4">
         <f>SUM(E9)</f>
@@ -917,10 +941,10 @@
         <v>30.778637999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C35" s="4">
         <f>E10</f>
@@ -928,10 +952,10 @@
       </c>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36" s="4">
         <f>SUM(C34:C35)</f>
@@ -939,12 +963,12 @@
       </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C38" s="4">
         <f>SUM(E13)</f>
@@ -952,9 +976,9 @@
       </c>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C39" s="4">
         <f>SUM(E14)</f>
@@ -962,9 +986,9 @@
       </c>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C40" s="4">
         <f>SUM(E15)</f>
@@ -978,19 +1002,19 @@
         <v>67.154999999999987</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C41" s="4"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C43" s="4">
         <f>SUM(E18)</f>
@@ -1004,10 +1028,10 @@
         <v>298.53450000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C44" s="4">
         <f>SUM(E19)</f>
@@ -1015,10 +1039,10 @@
       </c>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45" s="4">
         <f>SUM(C43:C44)</f>
@@ -1026,12 +1050,12 @@
       </c>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C47" s="4">
         <f>SUM(E22)</f>
@@ -1039,9 +1063,9 @@
       </c>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C48" s="4">
         <f>SUM(E23)</f>
@@ -1049,9 +1073,9 @@
       </c>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C49" s="4">
         <f>SUM(E24)</f>

</xml_diff>